<commit_message>
stashing changes before revert
</commit_message>
<xml_diff>
--- a/dist/HydraulicTestMethodsExplanation.xlsx
+++ b/dist/HydraulicTestMethodsExplanation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NYBackup\Docs\AquiferTestLocator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09788C84-085A-4838-9605-FA89203B624A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2678A1-1C10-4861-8A57-EAA00D419697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46C61083-6FF4-4D24-B30C-0E175E9DE95E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46C61083-6FF4-4D24-B30C-0E175E9DE95E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="375">
   <si>
     <t>AQA01</t>
   </si>
@@ -1150,13 +1150,19 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>AQS33</t>
+  </si>
+  <si>
+    <t>Bradbury and Rothschild (1985)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1168,6 +1174,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1193,12 +1206,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1513,23 +1527,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38301743-9306-40C1-BDA6-38ADD1DB5F90}">
-  <dimension ref="A1:J136"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="124.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="42.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" customWidth="1"/>
+    <col min="5" max="5" width="124.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>358</v>
       </c>
@@ -1543,7 +1557,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>361</v>
       </c>
@@ -1565,7 +1579,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>361</v>
       </c>
@@ -1587,7 +1601,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>361</v>
       </c>
@@ -1609,7 +1623,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>361</v>
       </c>
@@ -1631,7 +1645,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>361</v>
       </c>
@@ -1653,7 +1667,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -1675,7 +1689,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>361</v>
       </c>
@@ -1697,7 +1711,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>362</v>
       </c>
@@ -1719,7 +1733,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>367</v>
       </c>
@@ -1741,7 +1755,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>363</v>
       </c>
@@ -1763,7 +1777,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>363</v>
       </c>
@@ -1785,7 +1799,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>364</v>
       </c>
@@ -1807,7 +1821,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>364</v>
       </c>
@@ -1829,7 +1843,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>364</v>
       </c>
@@ -1851,7 +1865,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>364</v>
       </c>
@@ -1873,7 +1887,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>364</v>
       </c>
@@ -1895,7 +1909,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>364</v>
       </c>
@@ -1917,7 +1931,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>364</v>
       </c>
@@ -1939,7 +1953,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>364</v>
       </c>
@@ -1961,7 +1975,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>364</v>
       </c>
@@ -1983,7 +1997,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>364</v>
       </c>
@@ -2005,7 +2019,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>364</v>
       </c>
@@ -2027,7 +2041,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>361</v>
       </c>
@@ -2049,7 +2063,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>361</v>
       </c>
@@ -2071,7 +2085,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>361</v>
       </c>
@@ -2093,7 +2107,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>361</v>
       </c>
@@ -2115,7 +2129,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>361</v>
       </c>
@@ -2137,7 +2151,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>361</v>
       </c>
@@ -2159,7 +2173,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>361</v>
       </c>
@@ -2181,7 +2195,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>361</v>
       </c>
@@ -2203,7 +2217,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>361</v>
       </c>
@@ -2225,7 +2239,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>361</v>
       </c>
@@ -2247,7 +2261,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>361</v>
       </c>
@@ -2269,7 +2283,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>361</v>
       </c>
@@ -2291,7 +2305,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>361</v>
       </c>
@@ -2313,7 +2327,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>361</v>
       </c>
@@ -2335,7 +2349,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>361</v>
       </c>
@@ -2357,7 +2371,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>361</v>
       </c>
@@ -2379,7 +2393,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>361</v>
       </c>
@@ -2401,7 +2415,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>361</v>
       </c>
@@ -2423,7 +2437,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>361</v>
       </c>
@@ -2445,7 +2459,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>361</v>
       </c>
@@ -2467,7 +2481,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -2489,7 +2503,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>361</v>
       </c>
@@ -2511,7 +2525,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>361</v>
       </c>
@@ -2533,7 +2547,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>361</v>
       </c>
@@ -2555,7 +2569,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>361</v>
       </c>
@@ -2577,7 +2591,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>361</v>
       </c>
@@ -2599,7 +2613,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>361</v>
       </c>
@@ -2621,7 +2635,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>361</v>
       </c>
@@ -2643,7 +2657,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>361</v>
       </c>
@@ -2665,7 +2679,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>361</v>
       </c>
@@ -2687,7 +2701,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>361</v>
       </c>
@@ -2709,7 +2723,7 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>361</v>
       </c>
@@ -2731,7 +2745,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>361</v>
       </c>
@@ -2753,7 +2767,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>361</v>
       </c>
@@ -2775,7 +2789,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>361</v>
       </c>
@@ -2797,7 +2811,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -2819,7 +2833,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>361</v>
       </c>
@@ -2841,7 +2855,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>361</v>
       </c>
@@ -2863,7 +2877,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>365</v>
       </c>
@@ -2885,7 +2899,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>365</v>
       </c>
@@ -2907,7 +2921,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>365</v>
       </c>
@@ -2929,7 +2943,7 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>366</v>
       </c>
@@ -2951,7 +2965,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>366</v>
       </c>
@@ -2973,7 +2987,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>366</v>
       </c>
@@ -2995,7 +3009,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>366</v>
       </c>
@@ -3017,7 +3031,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>366</v>
       </c>
@@ -3039,7 +3053,7 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>366</v>
       </c>
@@ -3061,7 +3075,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>367</v>
       </c>
@@ -3083,7 +3097,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>367</v>
       </c>
@@ -3105,7 +3119,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>367</v>
       </c>
@@ -3127,7 +3141,7 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>367</v>
       </c>
@@ -3149,7 +3163,7 @@
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>368</v>
       </c>
@@ -3171,7 +3185,7 @@
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>368</v>
       </c>
@@ -3193,7 +3207,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>368</v>
       </c>
@@ -3215,7 +3229,7 @@
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>368</v>
       </c>
@@ -3237,7 +3251,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>369</v>
       </c>
@@ -3259,7 +3273,7 @@
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>369</v>
       </c>
@@ -3281,7 +3295,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>370</v>
       </c>
@@ -3303,7 +3317,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>370</v>
       </c>
@@ -3325,7 +3339,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>366</v>
       </c>
@@ -3347,7 +3361,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>366</v>
       </c>
@@ -3369,7 +3383,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>366</v>
       </c>
@@ -3391,7 +3405,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>366</v>
       </c>
@@ -3413,7 +3427,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>366</v>
       </c>
@@ -3435,7 +3449,7 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>366</v>
       </c>
@@ -3457,7 +3471,7 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>366</v>
       </c>
@@ -3479,7 +3493,7 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>366</v>
       </c>
@@ -3501,7 +3515,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>367</v>
       </c>
@@ -3523,7 +3537,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>367</v>
       </c>
@@ -3545,7 +3559,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>367</v>
       </c>
@@ -3567,7 +3581,7 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>367</v>
       </c>
@@ -3589,7 +3603,7 @@
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>369</v>
       </c>
@@ -3611,7 +3625,7 @@
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>369</v>
       </c>
@@ -3633,40 +3647,36 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>244</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>362</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>244</v>
@@ -3677,18 +3687,18 @@
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>362</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>244</v>
@@ -3699,18 +3709,18 @@
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>362</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>244</v>
@@ -3721,18 +3731,18 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>362</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>244</v>
@@ -3743,18 +3753,18 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>362</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>244</v>
@@ -3765,18 +3775,18 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>362</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>244</v>
@@ -3787,18 +3797,18 @@
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>362</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>244</v>
@@ -3809,18 +3819,18 @@
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>362</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>244</v>
@@ -3831,21 +3841,21 @@
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
@@ -3853,21 +3863,21 @@
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>363</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
@@ -3875,21 +3885,21 @@
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>363</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
@@ -3897,21 +3907,21 @@
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>363</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
@@ -3919,21 +3929,21 @@
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>363</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
@@ -3941,21 +3951,21 @@
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
@@ -3963,21 +3973,21 @@
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>371</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
@@ -3985,21 +3995,21 @@
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>371</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>281</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
@@ -4007,21 +4017,21 @@
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>371</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>281</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -4029,21 +4039,21 @@
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>371</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
@@ -4051,21 +4061,21 @@
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>371</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>291</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
@@ -4073,21 +4083,21 @@
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>371</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>291</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
@@ -4095,21 +4105,21 @@
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>371</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>291</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
@@ -4117,21 +4127,21 @@
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>371</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>291</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
@@ -4139,21 +4149,21 @@
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>371</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>291</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
@@ -4161,21 +4171,21 @@
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
@@ -4183,21 +4193,21 @@
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>363</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
@@ -4205,21 +4215,21 @@
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>363</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
@@ -4227,21 +4237,21 @@
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>363</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
@@ -4249,21 +4259,21 @@
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>363</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
@@ -4271,21 +4281,21 @@
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>363</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
@@ -4293,21 +4303,21 @@
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>363</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
@@ -4315,21 +4325,21 @@
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>363</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
@@ -4337,21 +4347,21 @@
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>363</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
@@ -4359,21 +4369,21 @@
       <c r="I129" s="1"/>
       <c r="J129" s="1"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -4381,21 +4391,21 @@
       <c r="I130" s="1"/>
       <c r="J130" s="1"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -4403,21 +4413,21 @@
       <c r="I131" s="1"/>
       <c r="J131" s="1"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>363</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>341</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -4425,21 +4435,21 @@
       <c r="I132" s="1"/>
       <c r="J132" s="1"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>363</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
@@ -4447,21 +4457,21 @@
       <c r="I133" s="1"/>
       <c r="J133" s="1"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>363</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>348</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
@@ -4469,21 +4479,21 @@
       <c r="I134" s="1"/>
       <c r="J134" s="1"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>363</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>348</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
@@ -4491,21 +4501,21 @@
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>363</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
@@ -4513,6 +4523,28 @@
       <c r="I136" s="1"/>
       <c r="J136" s="1"/>
     </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>363</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>